<commit_message>
added useCases and reviews
</commit_message>
<xml_diff>
--- a/Scrum/phase 2/Sprint 4/Sprint Backlog.xlsx
+++ b/Scrum/phase 2/Sprint 4/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letic\OneDrive\Ambiente de Trabalho\ES\ES_gantProject\Scrum\phase 2\Sprint 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762B8D67-C74C-426D-88D5-97A387867873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818C7895-3964-4CED-B9D1-1DAE89D85C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="552" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Task Description</t>
   </si>
@@ -78,13 +78,16 @@
   </si>
   <si>
     <t>Guilherme                 Leticia                         Joana</t>
+  </si>
+  <si>
+    <t>Leticia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +105,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -324,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -377,6 +388,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:F12"/>
+  <dimension ref="C2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,8 +683,8 @@
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
@@ -686,13 +698,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="15"/>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="3:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -704,7 +716,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="3:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
@@ -718,7 +730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -728,7 +740,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="3:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
@@ -738,27 +750,32 @@
       <c r="E8" s="6"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="3:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="3:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="3:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="3:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
@@ -768,7 +785,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="3:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:9" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -784,5 +801,6 @@
     <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>